<commit_message>
ingreso correo destino en xlsx y .txt con link del video
</commit_message>
<xml_diff>
--- a/datos_destino.xlsx
+++ b/datos_destino.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luise\Google Drive\Falabella\prueba_tecnica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FCD425-7A92-4D2D-85D4-BC716DA06773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC00C6DC-93CC-47F2-B359-9C03DEA3D2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,13 +48,13 @@
     <t>Mi nombre es Luis Eduardo Obando Bonilla, soy participante para la vacante de desarrollador RPA y este es el envío del .zip con el algoritmo desarrollado. Muchas gracias.</t>
   </si>
   <si>
-    <t>incapacidades.100digital@gmail.com</t>
-  </si>
-  <si>
     <t>Soy un mensaje enviado con python!</t>
   </si>
   <si>
     <t>C:/Users/luise/Downloads/demo-code.zip</t>
+  </si>
+  <si>
+    <t>jossandoval@falabella.com.co</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -454,7 +454,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -471,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5"/>
       <c r="E5" s="4"/>

</xml_diff>